<commit_message>
added config-file, error-log, requirements, and copy debug-log to stdout
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t xml:space="preserve">url</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">apple.com</t>
   </si>
   <si>
-    <t xml:space="preserve">http://adobe.co2аm/</t>
+    <t xml:space="preserve">http://adobe.com/</t>
   </si>
   <si>
     <t xml:space="preserve">adobe.com</t>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">t.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://telegram.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">телега</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -341,6 +350,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,10 +374,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -715,9 +728,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" display="http://adobe"/>
+    <hyperlink ref="A32" r:id="rId2" display="https://telegram.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>